<commit_message>
Fixed error from previous commit
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AB" sheetId="1" state="visible" r:id="rId2"/>
@@ -4027,48 +4027,48 @@
     <t xml:space="preserve">0.104, 0.494</t>
   </si>
   <si>
+    <t xml:space="preserve">0.687,-0.317</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.338, 0.076</t>
   </si>
   <si>
-    <t xml:space="preserve">0.687,-0.317</t>
+    <t xml:space="preserve">0.252,0.259</t>
   </si>
   <si>
     <t xml:space="preserve">0.254,0.019</t>
   </si>
   <si>
-    <t xml:space="preserve">0.252,0.259</t>
+    <t xml:space="preserve">0.765,-0.367</t>
   </si>
   <si>
     <t xml:space="preserve">0.340,-0.025</t>
   </si>
   <si>
-    <t xml:space="preserve">0.765,-0.367</t>
-  </si>
-  <si>
     <t xml:space="preserve">-0.078,-0.006</t>
   </si>
   <si>
     <t xml:space="preserve">0.311,0.300</t>
   </si>
   <si>
+    <t xml:space="preserve">0.688,-0.310</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.298,-0.138</t>
   </si>
   <si>
-    <t xml:space="preserve">0.688,-0.310</t>
+    <t xml:space="preserve">0.317,-0.259</t>
   </si>
   <si>
     <t xml:space="preserve">0.312,-0.00</t>
   </si>
   <si>
-    <t xml:space="preserve">0.317,-0.259</t>
+    <t xml:space="preserve">0.317,-0.2597</t>
   </si>
   <si>
     <t xml:space="preserve">0.312,0.001</t>
   </si>
   <si>
-    <t xml:space="preserve">0.317,-0.2597</t>
-  </si>
-  <si>
     <t xml:space="preserve">-0.021, -0.369</t>
   </si>
   <si>
@@ -4078,12 +4078,12 @@
     <t xml:space="preserve">0.023,-0.302</t>
   </si>
   <si>
+    <t xml:space="preserve">0.468, -0.238</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.212, 0</t>
   </si>
   <si>
-    <t xml:space="preserve">0.468, -0.238</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.040, -0.183</t>
   </si>
   <si>
@@ -4099,12 +4099,12 @@
     <t xml:space="preserve">0.007,-0.210</t>
   </si>
   <si>
+    <t xml:space="preserve">0.059,-0.143</t>
+  </si>
+  <si>
     <t xml:space="preserve">-0.062, -0.084</t>
   </si>
   <si>
-    <t xml:space="preserve">0.059,-0.143</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.011,-0.136</t>
   </si>
   <si>
@@ -4117,12 +4117,12 @@
     <t xml:space="preserve">0.063,-0.463</t>
   </si>
   <si>
+    <t xml:space="preserve">0.875, 0.669</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.887, -0.002</t>
   </si>
   <si>
-    <t xml:space="preserve">0.875, 0.669</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.176, 0.501</t>
   </si>
   <si>
@@ -4159,12 +4159,12 @@
     <t xml:space="preserve">-0.054,0.155</t>
   </si>
   <si>
+    <t xml:space="preserve">0.155,-0.025</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.030,0.00</t>
   </si>
   <si>
-    <t xml:space="preserve">0.155,-0.025</t>
-  </si>
-  <si>
     <t xml:space="preserve">-0.053,0.156</t>
   </si>
   <si>
@@ -4177,18 +4177,18 @@
     <t xml:space="preserve">0.011, -0.296</t>
   </si>
   <si>
+    <t xml:space="preserve">0.430,-0.512</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.247,0.004</t>
   </si>
   <si>
-    <t xml:space="preserve">0.430,-0.512</t>
+    <t xml:space="preserve">0.748,-0.331</t>
   </si>
   <si>
     <t xml:space="preserve">0.304,-0.108</t>
   </si>
   <si>
-    <t xml:space="preserve">0.748,-0.331</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.061, -0.274</t>
   </si>
   <si>
@@ -4204,12 +4204,12 @@
     <t xml:space="preserve">0.146,0.389</t>
   </si>
   <si>
+    <t xml:space="preserve">0.482,-0.210</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.200,-0.0</t>
   </si>
   <si>
-    <t xml:space="preserve">0.482,-0.210</t>
-  </si>
-  <si>
     <t xml:space="preserve">-0.029,-0.326</t>
   </si>
   <si>
@@ -4228,12 +4228,12 @@
     <t xml:space="preserve">0.226,-0.557</t>
   </si>
   <si>
+    <t xml:space="preserve">0.470,-0.500</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.227,-0.00</t>
   </si>
   <si>
-    <t xml:space="preserve">0.470,-0.500</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.258,0.617</t>
   </si>
   <si>
@@ -4276,12 +4276,12 @@
     <t xml:space="preserve">0.000,-0.346</t>
   </si>
   <si>
+    <t xml:space="preserve">0.442, 0.636</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.422, 0</t>
   </si>
   <si>
-    <t xml:space="preserve">0.442, 0.636</t>
-  </si>
-  <si>
     <t xml:space="preserve">-0.033,-0.145</t>
   </si>
   <si>
@@ -4297,12 +4297,12 @@
     <t xml:space="preserve">0.346,-0.339</t>
   </si>
   <si>
+    <t xml:space="preserve">1.432,-0.478</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.044,-0.000</t>
   </si>
   <si>
-    <t xml:space="preserve">1.432,-0.478</t>
-  </si>
-  <si>
     <t xml:space="preserve">-0.022,-0.303</t>
   </si>
   <si>
@@ -4315,21 +4315,21 @@
     <t xml:space="preserve">0.024, -0.345</t>
   </si>
   <si>
+    <t xml:space="preserve">0.236, 0.068</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.510, 0.629</t>
   </si>
   <si>
-    <t xml:space="preserve">0.236, 0.068</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.393,0.168</t>
   </si>
   <si>
+    <t xml:space="preserve">0.993,0.341</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.461,-0.00</t>
   </si>
   <si>
-    <t xml:space="preserve">0.993,0.341</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.160,0.470</t>
   </si>
   <si>
@@ -4345,27 +4345,27 @@
     <t xml:space="preserve">0.296,-0.379</t>
   </si>
   <si>
+    <t xml:space="preserve">910</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.554,-0.158</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.603,0.000</t>
   </si>
   <si>
-    <t xml:space="preserve">910</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.554,-0.158</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.000, -0.250</t>
   </si>
   <si>
     <t xml:space="preserve">0.372,-0.175</t>
   </si>
   <si>
+    <t xml:space="preserve">0.747,-0.205</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.396, 0.000</t>
   </si>
   <si>
-    <t xml:space="preserve">0.747,-0.205</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.000,-0.533</t>
   </si>
   <si>
@@ -4393,63 +4393,63 @@
     <t xml:space="preserve">-0.006, -0.342</t>
   </si>
   <si>
+    <t xml:space="preserve">-0.000, -0.411</t>
+  </si>
+  <si>
     <t xml:space="preserve">2.865, -0.066</t>
   </si>
   <si>
     <t xml:space="preserve">2.183, 0</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.000, -0.411</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.225, -0.600</t>
   </si>
   <si>
+    <t xml:space="preserve">0.898,0.451</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.291,0.014</t>
   </si>
   <si>
-    <t xml:space="preserve">0.898,0.451</t>
+    <t xml:space="preserve">0.403,0.361</t>
   </si>
   <si>
     <t xml:space="preserve">0.294,0.020</t>
   </si>
   <si>
-    <t xml:space="preserve">0.403,0.361</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.075,-0.180</t>
   </si>
   <si>
+    <t xml:space="preserve">0.322, 0.705</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.475, 0</t>
   </si>
   <si>
-    <t xml:space="preserve">0.322, 0.705</t>
+    <t xml:space="preserve">970</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.598,-0.591</t>
   </si>
   <si>
     <t xml:space="preserve">0.212,-0.104</t>
   </si>
   <si>
-    <t xml:space="preserve">970</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.598,-0.591</t>
+    <t xml:space="preserve">0.551,-0.530</t>
   </si>
   <si>
     <t xml:space="preserve">0.335,0.034</t>
   </si>
   <si>
-    <t xml:space="preserve">0.551,-0.530</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.652,-0.530</t>
   </si>
   <si>
+    <t xml:space="preserve">0.469,-0.565</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.187,-0.083</t>
   </si>
   <si>
-    <t xml:space="preserve">0.469,-0.565</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.105,0.417</t>
   </si>
   <si>
@@ -4483,12 +4483,12 @@
     <t xml:space="preserve">0.269,0.614</t>
   </si>
   <si>
+    <t xml:space="preserve">2.154, -0.449</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.521,0.00</t>
   </si>
   <si>
-    <t xml:space="preserve">2.154, -0.449</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.324, -0.583</t>
   </si>
   <si>
@@ -4513,13 +4513,16 @@
     <t xml:space="preserve">0.456,-0.524</t>
   </si>
   <si>
+    <t xml:space="preserve">2.850, -0.380</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.868, 0</t>
   </si>
   <si>
     <t xml:space="preserve">0.416, -0.001</t>
   </si>
   <si>
-    <t xml:space="preserve">2.850, -0.380</t>
+    <t xml:space="preserve">0.038, -0.171</t>
   </si>
   <si>
     <t xml:space="preserve">2.817, -0.200</t>
@@ -4528,9 +4531,6 @@
     <t xml:space="preserve">2.390, 0</t>
   </si>
   <si>
-    <t xml:space="preserve">0.038, -0.171</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.024,-0.415</t>
   </si>
   <si>
@@ -4540,57 +4540,57 @@
     <t xml:space="preserve">0.481,-0.547</t>
   </si>
   <si>
+    <t xml:space="preserve">1.001,0.574</t>
+  </si>
+  <si>
     <t xml:space="preserve">2.041,0.050</t>
   </si>
   <si>
-    <t xml:space="preserve">1.001,0.574</t>
+    <t xml:space="preserve">2.866, -0.723</t>
   </si>
   <si>
     <t xml:space="preserve">2.411, 0</t>
   </si>
   <si>
-    <t xml:space="preserve">2.866, -0.723</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.387,-0.00</t>
   </si>
   <si>
+    <t xml:space="preserve">1.002,0.636</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.417,-0.00</t>
   </si>
   <si>
-    <t xml:space="preserve">1.002,0.636</t>
+    <t xml:space="preserve">1.004, 0.573</t>
   </si>
   <si>
     <t xml:space="preserve">0.387, 0</t>
   </si>
   <si>
-    <t xml:space="preserve">1.004, 0.573</t>
+    <t xml:space="preserve">1.028, 0.682</t>
   </si>
   <si>
     <t xml:space="preserve">0.417, 0</t>
   </si>
   <si>
-    <t xml:space="preserve">1.028, 0.682</t>
+    <t xml:space="preserve">0.878,-0.593</t>
   </si>
   <si>
     <t xml:space="preserve">0.263, -0.001</t>
   </si>
   <si>
-    <t xml:space="preserve">0.878,-0.593</t>
+    <t xml:space="preserve">0.867,0.525</t>
   </si>
   <si>
     <t xml:space="preserve">0.383,0.003</t>
   </si>
   <si>
-    <t xml:space="preserve">0.867,0.525</t>
+    <t xml:space="preserve">0.434,-0.373</t>
   </si>
   <si>
     <t xml:space="preserve">0.410, 0.041</t>
   </si>
   <si>
-    <t xml:space="preserve">0.434,-0.373</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.217,-0.333</t>
   </si>
   <si>
@@ -4600,12 +4600,12 @@
     <t xml:space="preserve">0.578,0.255</t>
   </si>
   <si>
+    <t xml:space="preserve">0.484,-0.517</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.434,-0.047</t>
   </si>
   <si>
-    <t xml:space="preserve">0.484,-0.517</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.243,-0.0</t>
   </si>
   <si>
@@ -4618,28 +4618,28 @@
     <t xml:space="preserve">0.057, -0.400</t>
   </si>
   <si>
+    <t xml:space="preserve">sim_AP_f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.400, -0.281</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.714, -0.006</t>
   </si>
   <si>
-    <t xml:space="preserve">sim_AP_f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.400, -0.281</t>
+    <t xml:space="preserve">0.422,0.363</t>
   </si>
   <si>
     <t xml:space="preserve">0.250,0.032</t>
   </si>
   <si>
-    <t xml:space="preserve">0.422,0.363</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.322,0.631</t>
   </si>
   <si>
+    <t xml:space="preserve">0.387,-0.420</t>
+  </si>
+  <si>
     <t xml:space="preserve">0.579,-0.160</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.387,-0.420</t>
   </si>
   <si>
     <t xml:space="preserve">sim_APDS</t>
@@ -5063,10 +5063,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F892"/>
+  <dimension ref="A1:I892"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A578" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E604" activeCellId="0" sqref="E604"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A583" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A602" activeCellId="0" sqref="A602"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17073,6 +17073,9 @@
       <c r="F600" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G600" s="1"/>
+      <c r="H600" s="1"/>
+      <c r="I600" s="1"/>
     </row>
     <row r="601" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A601" s="1" t="s">
@@ -20286,8 +20289,8 @@
   </sheetPr>
   <dimension ref="A1:F892"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A574" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A600" activeCellId="0" sqref="A600"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A577" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E603" activeCellId="0" sqref="E603"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32277,7 +32280,7 @@
     </row>
     <row r="600" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A600" s="1" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="B600" s="1" t="s">
         <v>7</v>
@@ -40725,8 +40728,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A201" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F232" activeCellId="0" sqref="F232"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A210" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E236" activeCellId="0" sqref="E236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -45648,9 +45651,6 @@
       <c r="F240" s="1" t="s">
         <v>1332</v>
       </c>
-      <c r="I240" s="1" t="s">
-        <v>1333</v>
-      </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
@@ -45669,10 +45669,10 @@
         <v>1161</v>
       </c>
       <c r="F241" s="1" t="s">
+        <v>1333</v>
+      </c>
+      <c r="I241" s="1" t="s">
         <v>1334</v>
-      </c>
-      <c r="I241" s="1" t="s">
-        <v>1335</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45692,10 +45692,10 @@
         <v>1161</v>
       </c>
       <c r="F242" s="1" t="s">
+        <v>1335</v>
+      </c>
+      <c r="I242" s="1" t="s">
         <v>1336</v>
-      </c>
-      <c r="I242" s="1" t="s">
-        <v>1337</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45715,6 +45715,9 @@
         <v>1161</v>
       </c>
       <c r="F243" s="1" t="s">
+        <v>1337</v>
+      </c>
+      <c r="I243" s="1" t="s">
         <v>1338</v>
       </c>
     </row>
@@ -45737,9 +45740,6 @@
       <c r="F244" s="1" t="s">
         <v>1339</v>
       </c>
-      <c r="I244" s="1" t="s">
-        <v>1340</v>
-      </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
@@ -45758,10 +45758,10 @@
         <v>1161</v>
       </c>
       <c r="F245" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="I245" s="1" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45781,10 +45781,10 @@
         <v>1161</v>
       </c>
       <c r="F246" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="I246" s="1" t="s">
         <v>1342</v>
-      </c>
-      <c r="I246" s="1" t="s">
-        <v>1341</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45804,10 +45804,10 @@
         <v>1161</v>
       </c>
       <c r="F247" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="I247" s="1" t="s">
         <v>1342</v>
-      </c>
-      <c r="I247" s="1" t="s">
-        <v>1341</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45827,10 +45827,10 @@
         <v>1161</v>
       </c>
       <c r="F248" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="I248" s="1" t="s">
         <v>1342</v>
-      </c>
-      <c r="I248" s="1" t="s">
-        <v>1343</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45850,10 +45850,10 @@
         <v>1161</v>
       </c>
       <c r="F249" s="1" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I249" s="1" t="s">
         <v>1344</v>
-      </c>
-      <c r="I249" s="1" t="s">
-        <v>1345</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -45873,6 +45873,9 @@
         <v>1161</v>
       </c>
       <c r="F250" s="1" t="s">
+        <v>1345</v>
+      </c>
+      <c r="I250" s="1" t="s">
         <v>1346</v>
       </c>
     </row>
@@ -45955,9 +45958,6 @@
       <c r="F254" s="1" t="s">
         <v>1349</v>
       </c>
-      <c r="I254" s="1" t="s">
-        <v>1350</v>
-      </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="s">
@@ -45976,6 +45976,9 @@
         <v>1161</v>
       </c>
       <c r="F255" s="1" t="s">
+        <v>1350</v>
+      </c>
+      <c r="I255" s="1" t="s">
         <v>1351</v>
       </c>
     </row>
@@ -46098,9 +46101,6 @@
       <c r="F261" s="1" t="s">
         <v>1356</v>
       </c>
-      <c r="G261" s="1" t="s">
-        <v>1357</v>
-      </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
@@ -46119,10 +46119,10 @@
         <v>1161</v>
       </c>
       <c r="F262" s="1" t="s">
+        <v>1357</v>
+      </c>
+      <c r="G262" s="1" t="s">
         <v>1358</v>
-      </c>
-      <c r="G262" s="1" t="s">
-        <v>1357</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46142,6 +46142,9 @@
         <v>1161</v>
       </c>
       <c r="F263" s="1" t="s">
+        <v>1357</v>
+      </c>
+      <c r="G263" s="1" t="s">
         <v>1358</v>
       </c>
     </row>
@@ -46304,9 +46307,6 @@
       <c r="F271" s="1" t="s">
         <v>1360</v>
       </c>
-      <c r="I271" s="1" t="s">
-        <v>1363</v>
-      </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
@@ -46325,6 +46325,9 @@
         <v>1161</v>
       </c>
       <c r="F272" s="1" t="s">
+        <v>1363</v>
+      </c>
+      <c r="I272" s="1" t="s">
         <v>1364</v>
       </c>
     </row>
@@ -46647,9 +46650,6 @@
       <c r="F288" s="1" t="s">
         <v>1376</v>
       </c>
-      <c r="I288" s="1" t="s">
-        <v>1377</v>
-      </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
@@ -46668,6 +46668,9 @@
         <v>1161</v>
       </c>
       <c r="F289" s="1" t="s">
+        <v>1377</v>
+      </c>
+      <c r="I289" s="1" t="s">
         <v>1378</v>
       </c>
     </row>
@@ -46850,9 +46853,6 @@
       <c r="F298" s="1" t="s">
         <v>1231</v>
       </c>
-      <c r="I298" s="1" t="s">
-        <v>1383</v>
-      </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
@@ -46871,10 +46871,10 @@
         <v>1161</v>
       </c>
       <c r="F299" s="1" t="s">
+        <v>1383</v>
+      </c>
+      <c r="I299" s="1" t="s">
         <v>1384</v>
-      </c>
-      <c r="I299" s="1" t="s">
-        <v>1385</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -46894,6 +46894,9 @@
         <v>1161</v>
       </c>
       <c r="F300" s="1" t="s">
+        <v>1385</v>
+      </c>
+      <c r="I300" s="1" t="s">
         <v>1386</v>
       </c>
     </row>
@@ -47276,9 +47279,6 @@
       <c r="F319" s="1" t="s">
         <v>1146</v>
       </c>
-      <c r="I319" s="1" t="s">
-        <v>1392</v>
-      </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="1" t="s">
@@ -47297,6 +47297,9 @@
         <v>1161</v>
       </c>
       <c r="F320" s="1" t="s">
+        <v>1392</v>
+      </c>
+      <c r="I320" s="1" t="s">
         <v>1393</v>
       </c>
     </row>
@@ -47439,9 +47442,6 @@
       <c r="F327" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="I327" s="1" t="s">
-        <v>1400</v>
-      </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="1" t="s">
@@ -47460,6 +47460,9 @@
         <v>1161</v>
       </c>
       <c r="F328" s="1" t="s">
+        <v>1400</v>
+      </c>
+      <c r="I328" s="1" t="s">
         <v>1401</v>
       </c>
     </row>
@@ -47842,9 +47845,6 @@
       <c r="F347" s="1" t="s">
         <v>1415</v>
       </c>
-      <c r="I347" s="1" t="s">
-        <v>1416</v>
-      </c>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="1" t="s">
@@ -47863,6 +47863,9 @@
         <v>1161</v>
       </c>
       <c r="F348" s="1" t="s">
+        <v>1416</v>
+      </c>
+      <c r="I348" s="1" t="s">
         <v>1417</v>
       </c>
     </row>
@@ -48225,9 +48228,6 @@
       <c r="F366" s="1" t="s">
         <v>1349</v>
       </c>
-      <c r="I366" s="1" t="s">
-        <v>1423</v>
-      </c>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="1" t="s">
@@ -48246,6 +48246,9 @@
         <v>1161</v>
       </c>
       <c r="F367" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="I367" s="1" t="s">
         <v>1424</v>
       </c>
     </row>
@@ -48348,9 +48351,6 @@
       <c r="F372" s="1" t="s">
         <v>986</v>
       </c>
-      <c r="G372" s="1" t="s">
-        <v>1429</v>
-      </c>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="1" t="s">
@@ -48369,6 +48369,9 @@
         <v>1161</v>
       </c>
       <c r="F373" s="1" t="s">
+        <v>1429</v>
+      </c>
+      <c r="G373" s="1" t="s">
         <v>1430</v>
       </c>
     </row>
@@ -48391,9 +48394,6 @@
       <c r="F374" s="1" t="s">
         <v>1431</v>
       </c>
-      <c r="I374" s="1" t="s">
-        <v>1432</v>
-      </c>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="1" t="s">
@@ -48412,6 +48412,9 @@
         <v>1161</v>
       </c>
       <c r="F375" s="1" t="s">
+        <v>1432</v>
+      </c>
+      <c r="I375" s="1" t="s">
         <v>1433</v>
       </c>
     </row>
@@ -48514,9 +48517,6 @@
       <c r="F380" s="1" t="s">
         <v>1438</v>
       </c>
-      <c r="I380" s="1" t="s">
-        <v>1439</v>
-      </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="1" t="s">
@@ -48526,7 +48526,7 @@
         <v>9999</v>
       </c>
       <c r="C381" s="1" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D381" s="1" t="s">
         <v>3</v>
@@ -48535,6 +48535,9 @@
         <v>1161</v>
       </c>
       <c r="F381" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="I381" s="1" t="s">
         <v>1441</v>
       </c>
     </row>
@@ -48577,9 +48580,6 @@
       <c r="F383" s="1" t="s">
         <v>1443</v>
       </c>
-      <c r="I383" s="1" t="s">
-        <v>1444</v>
-      </c>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="1" t="s">
@@ -48598,6 +48598,9 @@
         <v>1161</v>
       </c>
       <c r="F384" s="1" t="s">
+        <v>1444</v>
+      </c>
+      <c r="I384" s="1" t="s">
         <v>1445</v>
       </c>
     </row>
@@ -48820,12 +48823,6 @@
       <c r="F395" s="1" t="s">
         <v>1448</v>
       </c>
-      <c r="G395" s="1" t="s">
-        <v>1455</v>
-      </c>
-      <c r="I395" s="1" t="s">
-        <v>1456</v>
-      </c>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="1" t="s">
@@ -48844,6 +48841,12 @@
         <v>1161</v>
       </c>
       <c r="F396" s="1" t="s">
+        <v>1455</v>
+      </c>
+      <c r="G396" s="1" t="s">
+        <v>1456</v>
+      </c>
+      <c r="I396" s="1" t="s">
         <v>1457</v>
       </c>
     </row>
@@ -48866,9 +48869,6 @@
       <c r="F397" s="1" t="s">
         <v>1458</v>
       </c>
-      <c r="I397" s="1" t="s">
-        <v>1459</v>
-      </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="1" t="s">
@@ -48887,10 +48887,10 @@
         <v>1161</v>
       </c>
       <c r="F398" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="I398" s="1" t="s">
         <v>1460</v>
-      </c>
-      <c r="I398" s="1" t="s">
-        <v>1461</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48910,6 +48910,9 @@
         <v>1161</v>
       </c>
       <c r="F399" s="1" t="s">
+        <v>1461</v>
+      </c>
+      <c r="I399" s="1" t="s">
         <v>1462</v>
       </c>
     </row>
@@ -48932,9 +48935,6 @@
       <c r="F400" s="1" t="s">
         <v>1463</v>
       </c>
-      <c r="I400" s="1" t="s">
-        <v>1464</v>
-      </c>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="1" t="s">
@@ -48953,10 +48953,10 @@
         <v>1161</v>
       </c>
       <c r="F401" s="1" t="s">
+        <v>1464</v>
+      </c>
+      <c r="I401" s="1" t="s">
         <v>1465</v>
-      </c>
-      <c r="I401" s="1" t="s">
-        <v>1016</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -48978,6 +48978,9 @@
       <c r="F402" s="1" t="s">
         <v>1015</v>
       </c>
+      <c r="I402" s="1" t="s">
+        <v>1016</v>
+      </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="1" t="s">
@@ -48998,9 +49001,6 @@
       <c r="F403" s="1" t="s">
         <v>1228</v>
       </c>
-      <c r="I403" s="1" t="s">
-        <v>1466</v>
-      </c>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="1" t="s">
@@ -49010,7 +49010,7 @@
         <v>9999</v>
       </c>
       <c r="C404" s="1" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="D404" s="1" t="s">
         <v>174</v>
@@ -49019,10 +49019,10 @@
         <v>1161</v>
       </c>
       <c r="F404" s="1" t="s">
+        <v>1467</v>
+      </c>
+      <c r="I404" s="1" t="s">
         <v>1468</v>
-      </c>
-      <c r="I404" s="1" t="s">
-        <v>1469</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49033,7 +49033,7 @@
         <v>1</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="D405" s="1" t="s">
         <v>48</v>
@@ -49042,10 +49042,10 @@
         <v>1161</v>
       </c>
       <c r="F405" s="1" t="s">
+        <v>1469</v>
+      </c>
+      <c r="I405" s="1" t="s">
         <v>1470</v>
-      </c>
-      <c r="I405" s="1" t="s">
-        <v>1469</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49056,7 +49056,7 @@
         <v>1</v>
       </c>
       <c r="C406" s="1" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="D406" s="1" t="s">
         <v>174</v>
@@ -49068,7 +49068,7 @@
         <v>1471</v>
       </c>
       <c r="I406" s="1" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49079,7 +49079,7 @@
         <v>9999</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="D407" s="1" t="s">
         <v>174</v>
@@ -49088,6 +49088,9 @@
         <v>1161</v>
       </c>
       <c r="F407" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="I407" s="1" t="s">
         <v>1473</v>
       </c>
     </row>
@@ -49490,9 +49493,6 @@
       <c r="F427" s="1" t="s">
         <v>1484</v>
       </c>
-      <c r="I427" s="1" t="s">
-        <v>1485</v>
-      </c>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="1" t="s">
@@ -49511,6 +49511,9 @@
         <v>1161</v>
       </c>
       <c r="F428" s="1" t="s">
+        <v>1485</v>
+      </c>
+      <c r="I428" s="1" t="s">
         <v>1486</v>
       </c>
     </row>
@@ -49673,12 +49676,6 @@
       <c r="F436" s="1" t="s">
         <v>1494</v>
       </c>
-      <c r="H436" s="1" t="s">
-        <v>1495</v>
-      </c>
-      <c r="I436" s="1" t="s">
-        <v>1496</v>
-      </c>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="2" t="s">
@@ -49697,13 +49694,13 @@
         <v>1161</v>
       </c>
       <c r="F437" s="1" t="s">
+        <v>1495</v>
+      </c>
+      <c r="H437" s="1" t="s">
+        <v>1496</v>
+      </c>
+      <c r="I437" s="1" t="s">
         <v>1497</v>
-      </c>
-      <c r="G437" s="1" t="s">
-        <v>1498</v>
-      </c>
-      <c r="I437" s="1" t="s">
-        <v>1499</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49723,6 +49720,12 @@
         <v>1161</v>
       </c>
       <c r="F438" s="1" t="s">
+        <v>1498</v>
+      </c>
+      <c r="G438" s="1" t="s">
+        <v>1499</v>
+      </c>
+      <c r="I438" s="1" t="s">
         <v>1500</v>
       </c>
     </row>
@@ -49825,9 +49828,6 @@
       <c r="F443" s="1" t="s">
         <v>1020</v>
       </c>
-      <c r="I443" s="1" t="s">
-        <v>1504</v>
-      </c>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="1" t="s">
@@ -49846,10 +49846,10 @@
         <v>1161</v>
       </c>
       <c r="F444" s="1" t="s">
+        <v>1504</v>
+      </c>
+      <c r="I444" s="1" t="s">
         <v>1505</v>
-      </c>
-      <c r="I444" s="1" t="s">
-        <v>1506</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49869,10 +49869,10 @@
         <v>1161</v>
       </c>
       <c r="F445" s="1" t="s">
+        <v>1506</v>
+      </c>
+      <c r="I445" s="1" t="s">
         <v>1507</v>
-      </c>
-      <c r="I445" s="1" t="s">
-        <v>1508</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49918,7 +49918,7 @@
         <v>907</v>
       </c>
       <c r="I447" s="1" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49938,10 +49938,10 @@
         <v>1161</v>
       </c>
       <c r="F448" s="1" t="s">
+        <v>1509</v>
+      </c>
+      <c r="I448" s="1" t="s">
         <v>1510</v>
-      </c>
-      <c r="I448" s="1" t="s">
-        <v>1508</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49964,7 +49964,7 @@
         <v>907</v>
       </c>
       <c r="I449" s="1" t="s">
-        <v>1511</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -49984,10 +49984,10 @@
         <v>1161</v>
       </c>
       <c r="F450" s="1" t="s">
+        <v>1511</v>
+      </c>
+      <c r="I450" s="1" t="s">
         <v>1512</v>
-      </c>
-      <c r="I450" s="1" t="s">
-        <v>1513</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50007,10 +50007,10 @@
         <v>1161</v>
       </c>
       <c r="F451" s="1" t="s">
+        <v>1513</v>
+      </c>
+      <c r="I451" s="1" t="s">
         <v>1514</v>
-      </c>
-      <c r="I451" s="1" t="s">
-        <v>1515</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50030,10 +50030,10 @@
         <v>1161</v>
       </c>
       <c r="F452" s="1" t="s">
+        <v>1515</v>
+      </c>
+      <c r="I452" s="1" t="s">
         <v>1516</v>
-      </c>
-      <c r="I452" s="1" t="s">
-        <v>1517</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50053,10 +50053,10 @@
         <v>1161</v>
       </c>
       <c r="F453" s="1" t="s">
+        <v>1517</v>
+      </c>
+      <c r="I453" s="1" t="s">
         <v>1518</v>
-      </c>
-      <c r="I453" s="1" t="s">
-        <v>1519</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50076,6 +50076,9 @@
         <v>1161</v>
       </c>
       <c r="F454" s="1" t="s">
+        <v>1519</v>
+      </c>
+      <c r="I454" s="1" t="s">
         <v>1520</v>
       </c>
     </row>
@@ -50158,9 +50161,6 @@
       <c r="F458" s="1" t="s">
         <v>1522</v>
       </c>
-      <c r="I458" s="1" t="s">
-        <v>1524</v>
-      </c>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="1" t="s">
@@ -50179,6 +50179,9 @@
         <v>1161</v>
       </c>
       <c r="F459" s="1" t="s">
+        <v>1524</v>
+      </c>
+      <c r="I459" s="1" t="s">
         <v>1525</v>
       </c>
     </row>
@@ -50201,9 +50204,6 @@
       <c r="F460" s="1" t="s">
         <v>1017</v>
       </c>
-      <c r="I460" s="1" t="s">
-        <v>1019</v>
-      </c>
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="1" t="s">
@@ -50224,6 +50224,9 @@
       <c r="F461" s="1" t="s">
         <v>1018</v>
       </c>
+      <c r="I461" s="1" t="s">
+        <v>1019</v>
+      </c>
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="1" t="s">
@@ -50304,9 +50307,6 @@
       <c r="F465" s="1" t="s">
         <v>1284</v>
       </c>
-      <c r="I465" s="1" t="s">
-        <v>1526</v>
-      </c>
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="1" t="s">
@@ -50327,6 +50327,9 @@
       <c r="F466" s="1" t="s">
         <v>1281</v>
       </c>
+      <c r="I466" s="1" t="s">
+        <v>1526</v>
+      </c>
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="1" t="s">
@@ -50387,9 +50390,6 @@
       <c r="F469" s="1" t="s">
         <v>1529</v>
       </c>
-      <c r="I469" s="1" t="s">
-        <v>1068</v>
-      </c>
     </row>
     <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="1" t="s">
@@ -50411,7 +50411,7 @@
         <v>1067</v>
       </c>
       <c r="I470" s="1" t="s">
-        <v>1530</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50428,13 +50428,13 @@
         <v>220</v>
       </c>
       <c r="E471" s="1" t="s">
+        <v>1530</v>
+      </c>
+      <c r="F471" s="1" t="s">
         <v>1531</v>
       </c>
-      <c r="F471" s="1" t="s">
+      <c r="I471" s="1" t="s">
         <v>1532</v>
-      </c>
-      <c r="I471" s="1" t="s">
-        <v>1533</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50451,9 +50451,12 @@
         <v>220</v>
       </c>
       <c r="E472" s="1" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="F472" s="1" t="s">
+        <v>1533</v>
+      </c>
+      <c r="I472" s="1" t="s">
         <v>1534</v>
       </c>
     </row>
@@ -50471,13 +50474,10 @@
         <v>48</v>
       </c>
       <c r="E473" s="1" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="F473" s="1" t="s">
         <v>1535</v>
-      </c>
-      <c r="I473" s="1" t="s">
-        <v>1536</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50494,9 +50494,12 @@
         <v>220</v>
       </c>
       <c r="E474" s="1" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="F474" s="1" t="s">
+        <v>1536</v>
+      </c>
+      <c r="I474" s="1" t="s">
         <v>1537</v>
       </c>
     </row>
@@ -50626,10 +50629,10 @@
         <v>1538</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>1467</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>1468</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>1466</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50649,10 +50652,10 @@
         <v>1538</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>1469</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>1470</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>1469</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50675,7 +50678,7 @@
         <v>1471</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50695,10 +50698,10 @@
         <v>1538</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>1473</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>1472</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50718,10 +50721,10 @@
         <v>1538</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>1337</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>1338</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>1337</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50761,7 +50764,7 @@
         <v>1538</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>1340</v>
@@ -50784,10 +50787,10 @@
         <v>1538</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>1342</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>1341</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50807,10 +50810,10 @@
         <v>1538</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>1342</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>1341</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50830,10 +50833,10 @@
         <v>1538</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>1342</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>1341</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50853,10 +50856,10 @@
         <v>1538</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>1343</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>1344</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>1343</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50879,7 +50882,7 @@
         <v>1539</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -50899,10 +50902,10 @@
         <v>1538</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>1459</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>1460</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>1459</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51025,10 +51028,10 @@
         <v>1538</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>1416</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>1417</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>1416</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51655,10 +51658,10 @@
         <v>1538</v>
       </c>
       <c r="F53" s="1" t="s">
+        <v>1504</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>1505</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>1504</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51747,10 +51750,10 @@
         <v>1538</v>
       </c>
       <c r="F57" s="1" t="s">
+        <v>1509</v>
+      </c>
+      <c r="I57" s="1" t="s">
         <v>1510</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>1509</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51816,7 +51819,7 @@
         <v>1538</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>1563</v>
@@ -51859,10 +51862,10 @@
         <v>1538</v>
       </c>
       <c r="F62" s="1" t="s">
+        <v>1511</v>
+      </c>
+      <c r="I62" s="1" t="s">
         <v>1512</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>1511</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -51882,10 +51885,10 @@
         <v>1538</v>
       </c>
       <c r="F63" s="1" t="s">
+        <v>1513</v>
+      </c>
+      <c r="I63" s="1" t="s">
         <v>1514</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>1513</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54030,10 +54033,10 @@
         <v>1538</v>
       </c>
       <c r="F162" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="I162" s="1" t="s">
         <v>1441</v>
-      </c>
-      <c r="I162" s="1" t="s">
-        <v>1439</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55456,8 +55459,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A113" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G133" activeCellId="0" sqref="G133"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A89" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D126" activeCellId="0" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -55526,10 +55529,10 @@
         <v>1633</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>1464</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>1465</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>1464</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55549,10 +55552,10 @@
         <v>1633</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>1517</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>1518</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>1517</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55572,10 +55575,10 @@
         <v>1633</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>1524</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>1525</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>1524</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55595,10 +55598,10 @@
         <v>1633</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>1467</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>1468</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>1466</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55618,10 +55621,10 @@
         <v>1633</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>1469</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>1470</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>1469</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55644,7 +55647,7 @@
         <v>1471</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -55664,10 +55667,10 @@
         <v>1633</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>1473</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>1472</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -57620,10 +57623,10 @@
         <v>1633</v>
       </c>
       <c r="F99" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="I99" s="1" t="s">
         <v>1441</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>1439</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added all_tanks sights for AB/RB Floppa
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AB" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,7 @@
     <sheet name="AP" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="APDS" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="LASER" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="ALL_TANKS" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16562" uniqueCount="1893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16583" uniqueCount="1894">
   <si>
     <t xml:space="preserve">uk_centurion_mk_5_avre_era</t>
   </si>
@@ -5706,6 +5707,9 @@
   </si>
   <si>
     <t xml:space="preserve">0.533, 0.730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all_tanks</t>
   </si>
 </sst>
 </file>
@@ -5873,11 +5877,11 @@
   </sheetPr>
   <dimension ref="A1:I789"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A659" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A716" activeCellId="0" sqref="A716"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A716" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G764" activeCellId="0" sqref="G764"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.65"/>
   </cols>
@@ -21639,7 +21643,7 @@
       <selection pane="topLeft" activeCell="A716" activeCellId="0" sqref="A716"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.65"/>
   </cols>
@@ -38094,10 +38098,10 @@
   <dimension ref="A1:I892"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A184" activeCellId="0" sqref="A184"/>
+      <selection pane="topLeft" activeCell="D185" activeCellId="0" sqref="D185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.65"/>
   </cols>
@@ -61821,7 +61825,7 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A185" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A185" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A231" activeCellId="0" sqref="A231"/>
     </sheetView>
   </sheetViews>
@@ -72260,4 +72264,182 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>622</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>982</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>983</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>984</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>986</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed 3 errors from it_btr80a
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3064,7 +3064,7 @@
     <t xml:space="preserve">it_leopard_bofors</t>
   </si>
   <si>
-    <t xml:space="preserve">it_btr_80a_hungary </t>
+    <t xml:space="preserve">it_btr_80a_hungary</t>
   </si>
   <si>
     <t xml:space="preserve">sw_k9_vidar</t>
@@ -6582,11 +6582,11 @@
   </sheetPr>
   <dimension ref="A1:I843"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A784" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G834" activeCellId="0" sqref="G834"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A796" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A821" activeCellId="0" sqref="A821"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.65"/>
   </cols>
@@ -23419,7 +23419,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="1" sqref="A821 A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24132,10 +24132,10 @@
   <dimension ref="A1:I902"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A799" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E846" activeCellId="0" sqref="E846"/>
+      <selection pane="topLeft" activeCell="A821" activeCellId="0" sqref="A821"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.65"/>
   </cols>
@@ -41276,10 +41276,10 @@
   <dimension ref="A1:I892"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A162" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E214" activeCellId="0" sqref="E214"/>
+      <selection pane="topLeft" activeCell="A207" activeCellId="1" sqref="A821 A207"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.65"/>
   </cols>
@@ -49408,7 +49408,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F53" activeCellId="0" sqref="F53"/>
+      <selection pane="topLeft" activeCell="F53" activeCellId="1" sqref="A821 F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -50465,7 +50465,7 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+      <selection pane="topLeft" activeCell="C40" activeCellId="1" sqref="A821 C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -55943,7 +55943,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A459" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O510" activeCellId="0" sqref="O510"/>
+      <selection pane="topLeft" activeCell="O510" activeCellId="1" sqref="A821 O510"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -66746,7 +66746,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A267" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B299" activeCellId="0" sqref="B299"/>
+      <selection pane="topLeft" activeCell="B299" activeCellId="1" sqref="A821 B299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -73364,7 +73364,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="A821 A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -78124,10 +78124,10 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="1" sqref="A821 C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>